<commit_message>
Add functionalities in Add Item
</commit_message>
<xml_diff>
--- a/item_details.xlsx
+++ b/item_details.xlsx
@@ -100,7 +100,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xml:space="preserve">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <b val="0"/>
       <i val="0"/>
@@ -125,6 +125,15 @@
       <strike val="0"/>
       <u val="none"/>
       <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <b val="0"/>
+      <i val="0"/>
+      <strike val="0"/>
+      <u val="none"/>
+      <sz val="14"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
     </font>
@@ -173,10 +182,10 @@
     <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="0">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="2" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="1" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
-    <xf xfId="0" fontId="0" numFmtId="0" fillId="0" borderId="1" applyFont="0" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
+    <xf xfId="0" fontId="3" numFmtId="0" fillId="0" borderId="1" applyFont="1" applyNumberFormat="0" applyFill="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" shrinkToFit="false"/>
     </xf>
   </cellXfs>

</xml_diff>